<commit_message>
aktivitettikaaviot ja selitykset lisätty kuvastoon
</commit_message>
<xml_diff>
--- a/Tietokannanmallintaminen.xlsx
+++ b/Tietokannanmallintaminen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xim\muistutussovellus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A1A39D-1E00-4C03-BBAF-459BCBA14020}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5832FDF9-6DFC-4E3F-AFDA-1CE1A9303409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" activeTab="2" xr2:uid="{61571C0B-95E2-4684-82D8-7B2B6CDD3356}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
   <si>
     <t>Tunniste</t>
   </si>
@@ -1703,6 +1703,157 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>493102</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Ryhmä 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F703A64B-380A-4F54-B31E-632D8969D62A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="10800000">
+          <a:off x="9220200" y="942975"/>
+          <a:ext cx="416902" cy="2181225"/>
+          <a:chOff x="1307123" y="676275"/>
+          <a:chExt cx="416902" cy="2181225"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Suora nuoliyhdysviiva 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A66396-EA1C-4393-A15B-4CD73BD3612C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1312252" y="2845777"/>
+            <a:ext cx="411773" cy="2199"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="17" name="Suora nuoliyhdysviiva 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA58660-1984-4B89-ADD9-02FD411AC42F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1307123" y="676275"/>
+            <a:ext cx="411773" cy="2199"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="18" name="Suora yhdysviiva 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC6A21D-F962-4570-AD3A-487F1C97FB4C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1319579" y="685800"/>
+            <a:ext cx="4396" cy="2171700"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2729,29 +2880,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B502A3A-5ACC-4FF4-88C3-BF4803BFC12F}">
-  <dimension ref="C1:O22"/>
+  <dimension ref="C1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19:M22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H1" s="7"/>
       <c r="I1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="11" t="s">
         <v>45</v>
@@ -2771,7 +2922,7 @@
       </c>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
         <v>46</v>
       </c>
@@ -2790,8 +2941,11 @@
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
@@ -2811,7 +2965,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2828,7 +2982,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>49</v>
       </c>
@@ -2845,7 +2999,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>50</v>
       </c>
@@ -2862,7 +3016,7 @@
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
         <v>56</v>
       </c>
@@ -2874,7 +3028,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
         <v>57</v>
       </c>
@@ -2886,14 +3040,14 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="M12" s="7"/>
       <c r="N12" s="24" t="s">
         <v>67</v>
       </c>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H13" s="7"/>
       <c r="I13" s="24" t="s">
         <v>87</v>
@@ -2905,7 +3059,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H14" s="8" t="s">
         <v>100</v>
       </c>
@@ -2917,7 +3071,7 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G15">
         <v>1</v>
       </c>
@@ -2932,7 +3086,7 @@
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H16" s="8" t="s">
         <v>86</v>
       </c>
@@ -2944,7 +3098,7 @@
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H17" s="9" t="s">
         <v>54</v>
       </c>
@@ -2956,7 +3110,7 @@
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H18" s="9" t="s">
         <v>55</v>
       </c>
@@ -2967,8 +3121,11 @@
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H19" s="9" t="s">
         <v>56</v>
       </c>
@@ -2980,21 +3137,21 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M20" s="9" t="s">
         <v>55</v>
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M21" s="9" t="s">
         <v>56</v>
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M22" s="9" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
luokkakaavio päivitetty, 3. normaalimuoto päivitetty
</commit_message>
<xml_diff>
--- a/Tietokannanmallintaminen.xlsx
+++ b/Tietokannanmallintaminen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xim\muistutussovellus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5832FDF9-6DFC-4E3F-AFDA-1CE1A9303409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC1555-0679-4570-89C7-3C2D8EA1B13B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" activeTab="2" xr2:uid="{61571C0B-95E2-4684-82D8-7B2B6CDD3356}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>Tunniste</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Käyttäjät</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>*kayttajatunnus</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Sahkoposti: str</t>
   </si>
   <si>
-    <t>Yritys_nimi: str</t>
-  </si>
-  <si>
     <t>GetList()</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>Hahmonimi: str</t>
   </si>
   <si>
-    <t xml:space="preserve">                *</t>
-  </si>
-  <si>
     <t>Suoritetut tehtävät</t>
   </si>
   <si>
@@ -359,10 +350,22 @@
     <t>Tavoite: str</t>
   </si>
   <si>
-    <t>Tavoite_suoritettu: bool</t>
-  </si>
-  <si>
     <t>Pvm: dt</t>
+  </si>
+  <si>
+    <t>1, *</t>
+  </si>
+  <si>
+    <t>1,*</t>
+  </si>
+  <si>
+    <t>TavoiteSuoritettu: bool</t>
+  </si>
+  <si>
+    <t>Animaatio: ?</t>
+  </si>
+  <si>
+    <t>YritysNimi: str</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,6 +604,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20 % - Aksentti5" xfId="2" builtinId="46"/>
@@ -1499,157 +1505,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>550252</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Ryhmä 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3790950" y="762000"/>
-          <a:ext cx="416902" cy="2181225"/>
-          <a:chOff x="1307123" y="676275"/>
-          <a:chExt cx="416902" cy="2181225"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="Suora nuoliyhdysviiva 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD482C4-C207-4D04-B930-9B73D861913A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1307123" y="676275"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1319579" y="685800"/>
-            <a:ext cx="4396" cy="2171700"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -1712,9 +1567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>493102</xdr:colOff>
+      <xdr:colOff>487973</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1730,9 +1585,9 @@
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
           <a:off x="9220200" y="942975"/>
-          <a:ext cx="416902" cy="2181225"/>
-          <a:chOff x="1307123" y="676275"/>
-          <a:chExt cx="416902" cy="2181225"/>
+          <a:ext cx="411773" cy="2171700"/>
+          <a:chOff x="1312252" y="685800"/>
+          <a:chExt cx="411773" cy="2171700"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -1749,44 +1604,6 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="17" name="Suora nuoliyhdysviiva 16">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA58660-1984-4B89-ADD9-02FD411AC42F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1307123" y="676275"/>
             <a:ext cx="411773" cy="2199"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -1852,6 +1669,226 @@
         </xdr:style>
       </xdr:cxnSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>138479</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Ryhmä 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83CC1DF2-2428-4AD5-A20B-212FA7573C5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3796079" y="771525"/>
+          <a:ext cx="433021" cy="2171700"/>
+          <a:chOff x="3796079" y="771525"/>
+          <a:chExt cx="433021" cy="2171700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="9" name="Ryhmä 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="3796079" y="771525"/>
+            <a:ext cx="411773" cy="2171700"/>
+            <a:chOff x="1312252" y="685800"/>
+            <a:chExt cx="411773" cy="2171700"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1312252" y="2845777"/>
+              <a:ext cx="411773" cy="2199"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1319579" y="685800"/>
+              <a:ext cx="4396" cy="2171700"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Suora yhdysviiva 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A9A57D-9EA7-4D54-948E-2CC1C5E4AFAD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3800475" y="781050"/>
+            <a:ext cx="428625" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>43229</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>471854</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Suora yhdysviiva 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F887DB22-18CF-4A79-B6C3-B854C70BA33D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9187229" y="3105150"/>
+          <a:ext cx="428625" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2203,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -2221,7 +2258,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,10 +2313,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
@@ -2290,7 +2327,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2415,7 +2452,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2423,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -2441,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2449,7 +2486,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2467,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2475,7 +2512,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -2485,13 +2522,13 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2499,16 +2536,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" t="s">
         <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2516,7 +2553,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -2534,7 +2571,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -2552,13 +2589,13 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2685,7 +2722,7 @@
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J2" s="22"/>
       <c r="K2" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L2" s="22"/>
     </row>
@@ -2696,76 +2733,76 @@
       </c>
       <c r="F3" s="21"/>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -2773,103 +2810,103 @@
     <row r="12" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="19"/>
       <c r="E12" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F12" s="21"/>
       <c r="J12" s="19"/>
       <c r="K12" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L12" s="21"/>
     </row>
     <row r="13" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2920,7 @@
   <dimension ref="C1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,7 +2934,7 @@
     </row>
     <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -2905,137 +2942,137 @@
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="7"/>
       <c r="H3" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="12"/>
-      <c r="K3" t="s">
-        <v>28</v>
+      <c r="K3" s="2">
+        <v>1</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="G4" t="s">
-        <v>102</v>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="2">
-        <v>1</v>
+      <c r="P4" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="L5">
-        <v>1</v>
+      <c r="L5" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="H6" s="10" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="M6" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="M7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="M8" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="M9" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="M10" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -3043,30 +3080,30 @@
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="M12" s="7"/>
       <c r="N12" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H13" s="7"/>
       <c r="I13" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J13" s="7"/>
       <c r="M13" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="M14" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -3076,31 +3113,31 @@
         <v>1</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="M15" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H16" s="8" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="M16" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H17" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -3112,48 +3149,48 @@
     </row>
     <row r="18" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="M18" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H19" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="M19" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M20" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M21" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M22" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>

</xml_diff>

<commit_message>
luokkakaavio päivitetty, 3. normaalimuoto päivitetty (#29)
</commit_message>
<xml_diff>
--- a/Tietokannanmallintaminen.xlsx
+++ b/Tietokannanmallintaminen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xim\muistutussovellus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5832FDF9-6DFC-4E3F-AFDA-1CE1A9303409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC1555-0679-4570-89C7-3C2D8EA1B13B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" activeTab="2" xr2:uid="{61571C0B-95E2-4684-82D8-7B2B6CDD3356}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>Tunniste</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Käyttäjät</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>*kayttajatunnus</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Sahkoposti: str</t>
   </si>
   <si>
-    <t>Yritys_nimi: str</t>
-  </si>
-  <si>
     <t>GetList()</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>Hahmonimi: str</t>
   </si>
   <si>
-    <t xml:space="preserve">                *</t>
-  </si>
-  <si>
     <t>Suoritetut tehtävät</t>
   </si>
   <si>
@@ -359,10 +350,22 @@
     <t>Tavoite: str</t>
   </si>
   <si>
-    <t>Tavoite_suoritettu: bool</t>
-  </si>
-  <si>
     <t>Pvm: dt</t>
+  </si>
+  <si>
+    <t>1, *</t>
+  </si>
+  <si>
+    <t>1,*</t>
+  </si>
+  <si>
+    <t>TavoiteSuoritettu: bool</t>
+  </si>
+  <si>
+    <t>Animaatio: ?</t>
+  </si>
+  <si>
+    <t>YritysNimi: str</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,6 +604,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20 % - Aksentti5" xfId="2" builtinId="46"/>
@@ -1499,157 +1505,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>550252</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Ryhmä 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3790950" y="762000"/>
-          <a:ext cx="416902" cy="2181225"/>
-          <a:chOff x="1307123" y="676275"/>
-          <a:chExt cx="416902" cy="2181225"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="Suora nuoliyhdysviiva 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD482C4-C207-4D04-B930-9B73D861913A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1307123" y="676275"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1319579" y="685800"/>
-            <a:ext cx="4396" cy="2171700"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -1712,9 +1567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>493102</xdr:colOff>
+      <xdr:colOff>487973</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1730,9 +1585,9 @@
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
           <a:off x="9220200" y="942975"/>
-          <a:ext cx="416902" cy="2181225"/>
-          <a:chOff x="1307123" y="676275"/>
-          <a:chExt cx="416902" cy="2181225"/>
+          <a:ext cx="411773" cy="2171700"/>
+          <a:chOff x="1312252" y="685800"/>
+          <a:chExt cx="411773" cy="2171700"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -1749,44 +1604,6 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="17" name="Suora nuoliyhdysviiva 16">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA58660-1984-4B89-ADD9-02FD411AC42F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1307123" y="676275"/>
             <a:ext cx="411773" cy="2199"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -1852,6 +1669,226 @@
         </xdr:style>
       </xdr:cxnSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>138479</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Ryhmä 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83CC1DF2-2428-4AD5-A20B-212FA7573C5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3796079" y="771525"/>
+          <a:ext cx="433021" cy="2171700"/>
+          <a:chOff x="3796079" y="771525"/>
+          <a:chExt cx="433021" cy="2171700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="9" name="Ryhmä 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="3796079" y="771525"/>
+            <a:ext cx="411773" cy="2171700"/>
+            <a:chOff x="1312252" y="685800"/>
+            <a:chExt cx="411773" cy="2171700"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1312252" y="2845777"/>
+              <a:ext cx="411773" cy="2199"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1319579" y="685800"/>
+              <a:ext cx="4396" cy="2171700"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Suora yhdysviiva 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A9A57D-9EA7-4D54-948E-2CC1C5E4AFAD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3800475" y="781050"/>
+            <a:ext cx="428625" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>43229</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>471854</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Suora yhdysviiva 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F887DB22-18CF-4A79-B6C3-B854C70BA33D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9187229" y="3105150"/>
+          <a:ext cx="428625" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2203,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -2221,7 +2258,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,10 +2313,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
@@ -2290,7 +2327,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2415,7 +2452,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2423,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -2441,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2449,7 +2486,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2467,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2475,7 +2512,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -2485,13 +2522,13 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2499,16 +2536,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" t="s">
         <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2516,7 +2553,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -2534,7 +2571,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -2552,13 +2589,13 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2685,7 +2722,7 @@
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J2" s="22"/>
       <c r="K2" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L2" s="22"/>
     </row>
@@ -2696,76 +2733,76 @@
       </c>
       <c r="F3" s="21"/>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -2773,103 +2810,103 @@
     <row r="12" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="19"/>
       <c r="E12" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F12" s="21"/>
       <c r="J12" s="19"/>
       <c r="K12" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L12" s="21"/>
     </row>
     <row r="13" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2920,7 @@
   <dimension ref="C1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,7 +2934,7 @@
     </row>
     <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -2905,137 +2942,137 @@
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="7"/>
       <c r="H3" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="12"/>
-      <c r="K3" t="s">
-        <v>28</v>
+      <c r="K3" s="2">
+        <v>1</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="G4" t="s">
-        <v>102</v>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="2">
-        <v>1</v>
+      <c r="P4" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="L5">
-        <v>1</v>
+      <c r="L5" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="H6" s="10" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="M6" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="M7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="M8" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="M9" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="M10" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -3043,30 +3080,30 @@
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="M12" s="7"/>
       <c r="N12" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H13" s="7"/>
       <c r="I13" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J13" s="7"/>
       <c r="M13" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="M14" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -3076,31 +3113,31 @@
         <v>1</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="M15" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H16" s="8" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="M16" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H17" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -3112,48 +3149,48 @@
     </row>
     <row r="18" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="M18" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H19" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="M19" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M20" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M21" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.25">
       <c r="M22" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>

</xml_diff>

<commit_message>
tietokannanmallit päivitetty ja siirretty kuvastoihin
</commit_message>
<xml_diff>
--- a/Tietokannanmallintaminen.xlsx
+++ b/Tietokannanmallintaminen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xim\muistutussovellus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC1555-0679-4570-89C7-3C2D8EA1B13B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82DEE55-5532-4202-9A6F-8AECB40E36EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" activeTab="2" xr2:uid="{61571C0B-95E2-4684-82D8-7B2B6CDD3356}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="133">
   <si>
     <t>Tunniste</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Käyttäjän nimi</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>Katti Matikainen</t>
   </si>
   <si>
@@ -167,45 +164,6 @@
     <t>Sijoituksia voidaan lajitella päivämäärän mukaan</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Käyttäjätunnus: str</t>
-  </si>
-  <si>
-    <t>Salasana: str</t>
-  </si>
-  <si>
-    <t>Autherize()</t>
-  </si>
-  <si>
-    <t>LogOut()</t>
-  </si>
-  <si>
-    <t>LoggedOut()</t>
-  </si>
-  <si>
-    <t>Tunnus: int</t>
-  </si>
-  <si>
-    <t>Sahkoposti: str</t>
-  </si>
-  <si>
-    <t>GetList()</t>
-  </si>
-  <si>
-    <t>GetSingleGroup()</t>
-  </si>
-  <si>
-    <t>Update()</t>
-  </si>
-  <si>
-    <t>Delete()</t>
-  </si>
-  <si>
-    <t>Pisteet: int</t>
-  </si>
-  <si>
     <t>int/10</t>
   </si>
   <si>
@@ -263,12 +221,6 @@
     <t>Tavoite suoritettu</t>
   </si>
   <si>
-    <t>Bool</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Tarkistaa onko tavoitteen pisteet saavutettu</t>
   </si>
   <si>
@@ -329,43 +281,157 @@
     <t>*tavoite_id</t>
   </si>
   <si>
-    <t>Hahmotunnus: str</t>
-  </si>
-  <si>
-    <t>Hahmonimi: str</t>
-  </si>
-  <si>
-    <t>Suoritetut tehtävät</t>
-  </si>
-  <si>
-    <t>Id: int</t>
-  </si>
-  <si>
-    <t>Tavoite: int</t>
-  </si>
-  <si>
-    <t>Suorituskerrat: int</t>
-  </si>
-  <si>
-    <t>Tavoite: str</t>
-  </si>
-  <si>
-    <t>Pvm: dt</t>
-  </si>
-  <si>
-    <t>1, *</t>
-  </si>
-  <si>
-    <t>1,*</t>
-  </si>
-  <si>
-    <t>TavoiteSuoritettu: bool</t>
-  </si>
-  <si>
-    <t>Animaatio: ?</t>
-  </si>
-  <si>
-    <t>YritysNimi: str</t>
+    <t>Linkki animaation sijaintiin</t>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t>www.linkki.fi/animaatiot/juoksu.aep</t>
+  </si>
+  <si>
+    <t>Uusi päivä</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Onko uusi päivä vai ei?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarkistaa, onko käyttäjä admin </t>
+  </si>
+  <si>
+    <t>Rekisteröintikoodi</t>
+  </si>
+  <si>
+    <t>Koodi, jolla pelaaja rekisteröityy yrityksensä pelialustalle</t>
+  </si>
+  <si>
+    <t>Pakollinen tehtävä</t>
+  </si>
+  <si>
+    <t>Tarkistaa, onko tehtävä pakollinen</t>
+  </si>
+  <si>
+    <t>Tavoitemäärä</t>
+  </si>
+  <si>
+    <t>Tehtävän tavoitemäärä</t>
+  </si>
+  <si>
+    <t>Viimeinen muokkaus</t>
+  </si>
+  <si>
+    <t>Tarkistaa, milloin pelaaja on viimeeksi suorittanut tehtävää</t>
+  </si>
+  <si>
+    <t>Hahmot</t>
+  </si>
+  <si>
+    <t>nimi: nvarchar</t>
+  </si>
+  <si>
+    <t>PK hahmo_id: int</t>
+  </si>
+  <si>
+    <t>animaatio1: nvarchar</t>
+  </si>
+  <si>
+    <t>animaatio2: nvarchar</t>
+  </si>
+  <si>
+    <t>animaatio3: nvarchar</t>
+  </si>
+  <si>
+    <t>Hae()</t>
+  </si>
+  <si>
+    <t>HaeKaikki()</t>
+  </si>
+  <si>
+    <t>Muokkaa()</t>
+  </si>
+  <si>
+    <t>Poista()</t>
+  </si>
+  <si>
+    <t>PK käyttäjä_id: int</t>
+  </si>
+  <si>
+    <t>FK hahmo_id: int</t>
+  </si>
+  <si>
+    <t>etunimi: nvarchar</t>
+  </si>
+  <si>
+    <t>sukunimi: nvarchar</t>
+  </si>
+  <si>
+    <t>salasana: nvarchar</t>
+  </si>
+  <si>
+    <t>sähköposti: nvarchar</t>
+  </si>
+  <si>
+    <t>rekisteröintikoodi: in</t>
+  </si>
+  <si>
+    <t>uusipäivä: bit</t>
+  </si>
+  <si>
+    <t>yritys: nvarchar</t>
+  </si>
+  <si>
+    <t>admin: bit</t>
+  </si>
+  <si>
+    <t>HaeRyhmä()</t>
+  </si>
+  <si>
+    <t>ValitutTehtävät</t>
+  </si>
+  <si>
+    <t>PK valitutteht_id: int</t>
+  </si>
+  <si>
+    <t>FK käyttäjä_id: int</t>
+  </si>
+  <si>
+    <t>FK tehtävä_id: int</t>
+  </si>
+  <si>
+    <t>pisteet: int</t>
+  </si>
+  <si>
+    <t>viimeinenmuokkaus: datetime</t>
+  </si>
+  <si>
+    <t>ei pidä paikkansa. Oikea er-malli suunnittelukuvastossa.</t>
+  </si>
+  <si>
+    <t>PK tehtävä_id: int</t>
+  </si>
+  <si>
+    <t>pistemäärä: int</t>
+  </si>
+  <si>
+    <t>tavoitemäärä: int</t>
+  </si>
+  <si>
+    <t>päivämäärä: datetime</t>
+  </si>
+  <si>
+    <t>pakollinen: bit</t>
+  </si>
+  <si>
+    <t>yrityskoodi: int</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -445,7 +511,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,8 +555,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -550,6 +634,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -561,7 +654,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,18 +670,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -602,9 +683,44 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1229,51 +1345,48 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604801</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Suora yhdysviiva 2">
+        <xdr:cNvPr id="17" name="Yhdistin: Kulma 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B54356-0BB7-4E2F-AE12-AFFB9466CF84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D06900B2-1947-4007-969C-57C6CCE86B0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1228725" y="962025"/>
-          <a:ext cx="1828800" cy="9525"/>
+        <a:xfrm rot="10800000">
+          <a:off x="3043201" y="296776"/>
+          <a:ext cx="1224000" cy="1332000"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1284,106 +1397,48 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>607201</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Suora yhdysviiva 6">
+        <xdr:cNvPr id="29" name="Yhdistin: Kulma 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C23F0CE-D645-4299-868A-F84C11FB3328}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1726CA-9CF4-4066-8346-6F4555BF192A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4257675" y="1152525"/>
-          <a:ext cx="1828800" cy="9525"/>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="6093601" y="502276"/>
+          <a:ext cx="612000" cy="936000"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Suora yhdysviiva 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B0316DD-4D2F-4165-8491-2882DFDDED78}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="1533525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1395,493 +1450,106 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Vinoneliö 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3615AA-0D14-4524-AA92-596282C40752}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="371475"/>
+          <a:ext cx="276225" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>607201</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Yhdistin: Kulma 9">
+        <xdr:cNvPr id="31" name="Yhdistin: Kulma 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9008C204-0973-4FF2-BD6F-AD49F8D43BDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4DA4F5-336A-4919-A968-44B7CDAAD30E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6105525" y="571500"/>
-          <a:ext cx="1219200" cy="571500"/>
+        <a:xfrm rot="10800000">
+          <a:off x="8532001" y="662251"/>
+          <a:ext cx="612000" cy="576000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Suora yhdysviiva 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7717D20-59E4-4E74-9BB9-49CDB3F37E27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4267200" y="3057525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Suora yhdysviiva 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E1CEC3-A659-408D-9F9C-70ED042D4045}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7305675" y="3438525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>487973</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Ryhmä 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F703A64B-380A-4F54-B31E-632D8969D62A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm rot="10800000">
-          <a:off x="9220200" y="942975"/>
-          <a:ext cx="411773" cy="2171700"/>
-          <a:chOff x="1312252" y="685800"/>
-          <a:chExt cx="411773" cy="2171700"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="16" name="Suora nuoliyhdysviiva 15">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A66396-EA1C-4393-A15B-4CD73BD3612C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="18" name="Suora yhdysviiva 17">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC6A21D-F962-4570-AD3A-487F1C97FB4C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1319579" y="685800"/>
-            <a:ext cx="4396" cy="2171700"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>138479</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="22" name="Ryhmä 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83CC1DF2-2428-4AD5-A20B-212FA7573C5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3796079" y="771525"/>
-          <a:ext cx="433021" cy="2171700"/>
-          <a:chOff x="3796079" y="771525"/>
-          <a:chExt cx="433021" cy="2171700"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="9" name="Ryhmä 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="3796079" y="771525"/>
-            <a:ext cx="411773" cy="2171700"/>
-            <a:chOff x="1312252" y="685800"/>
-            <a:chExt cx="411773" cy="2171700"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1312252" y="2845777"/>
-              <a:ext cx="411773" cy="2199"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1319579" y="685800"/>
-              <a:ext cx="4396" cy="2171700"/>
-            </a:xfrm>
-            <a:prstGeom prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-      </xdr:grpSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="4" name="Suora yhdysviiva 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A9A57D-9EA7-4D54-948E-2CC1C5E4AFAD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3800475" y="781050"/>
-            <a:ext cx="428625" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>43229</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>471854</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Suora yhdysviiva 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F887DB22-18CF-4A79-B6C3-B854C70BA33D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9187229" y="3105150"/>
-          <a:ext cx="428625" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
+        <a:lnRef idx="3">
           <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
           <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="2">
           <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -2193,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D048614-1B1B-4BED-86DE-CDA5E2BCD1F2}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +1872,7 @@
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="73.42578125" customWidth="1"/>
   </cols>
@@ -2240,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -2258,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2269,20 +1937,18 @@
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3">
         <v>30</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2290,22 +1956,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2313,21 +1976,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="3">
-        <v>6.5740740740740738E-2</v>
+      <c r="F5" s="16">
+        <v>43984</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2335,22 +1998,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2358,7 +2018,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -2376,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,7 +2044,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -2402,7 +2062,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,23 +2070,21 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3">
         <v>50</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2434,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2451,8 +2109,8 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>67</v>
+      <c r="H10" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2460,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -2471,14 +2129,14 @@
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>1234567890</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2486,7 +2144,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2497,14 +2155,14 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>987654321</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2512,23 +2170,23 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3">
         <v>150</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2536,16 +2194,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
+        <v>86</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2553,7 +2211,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -2571,7 +2229,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2579,98 +2237,178 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2">
         <v>30</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="2">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2">
+        <v>67890</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="A22" s="2">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="16">
+        <v>43992</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -2695,18 +2433,19 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" xr:uid="{480B066D-8DD9-4683-9ED8-6C2FC49271C4}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{0793E14C-77EC-4043-A5C9-ED6F6A97FA1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3ED8FE-25BB-46DF-9687-5EE052BFD54B}">
-  <dimension ref="D2:L18"/>
+  <dimension ref="D1:L18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,194 +2458,199 @@
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="22"/>
-      <c r="K2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" s="22"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="19"/>
-      <c r="E3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="21"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13"/>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>35</v>
+      <c r="E4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="15"/>
+        <v>71</v>
+      </c>
+      <c r="K9" s="7"/>
     </row>
     <row r="11" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="19"/>
-      <c r="E12" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="21"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="21"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="16" t="s">
+      <c r="E14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="16" t="s">
+      <c r="E15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="L15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2917,285 +2661,384 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B502A3A-5ACC-4FF4-88C3-BF4803BFC12F}">
-  <dimension ref="C1:P22"/>
+  <dimension ref="C1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H1" s="7"/>
-      <c r="I1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-      <c r="D3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="H3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="2">
+    <row r="1" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="24"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="21">
         <v>1</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="G4">
+      <c r="G3" s="20"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="32"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="21">
         <v>1</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="M4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="2" t="s">
+      <c r="L9" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="L5" s="26" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20">
+        <v>1</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H11" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="P11" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H12" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="P12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H13" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="P13" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H14" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="P14" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="P15" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H16" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="P16" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="H6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="M6" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="M7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="M8" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="M9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="M10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="M12" s="7"/>
-      <c r="N12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H13" s="7"/>
-      <c r="I13" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="M13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H14" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="M14" s="8" t="s">
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+    </row>
+    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H17" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="P17" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+    </row>
+    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H18" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="M15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="M16" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="M17" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="M18" s="8" t="s">
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H19" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" t="s">
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H22" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="M19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L2:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
tietokannanmallit päivitetty ja siirretty kuvastoihin (#85)
* bgn animaatio

* juoksuanimaatio korjattu

* tönäisyanimaatio korjattu

* kaatumisanimaatio lisätty

* ilotulitus2-animaatio

* puuttuvat bg-kuvat lisätty

* tietokannanmallit päivitetty ja siirretty kuvastoihin
</commit_message>
<xml_diff>
--- a/Tietokannanmallintaminen.xlsx
+++ b/Tietokannanmallintaminen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xim\muistutussovellus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC1555-0679-4570-89C7-3C2D8EA1B13B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82DEE55-5532-4202-9A6F-8AECB40E36EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" activeTab="2" xr2:uid="{61571C0B-95E2-4684-82D8-7B2B6CDD3356}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="133">
   <si>
     <t>Tunniste</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Käyttäjän nimi</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>Katti Matikainen</t>
   </si>
   <si>
@@ -167,45 +164,6 @@
     <t>Sijoituksia voidaan lajitella päivämäärän mukaan</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Käyttäjätunnus: str</t>
-  </si>
-  <si>
-    <t>Salasana: str</t>
-  </si>
-  <si>
-    <t>Autherize()</t>
-  </si>
-  <si>
-    <t>LogOut()</t>
-  </si>
-  <si>
-    <t>LoggedOut()</t>
-  </si>
-  <si>
-    <t>Tunnus: int</t>
-  </si>
-  <si>
-    <t>Sahkoposti: str</t>
-  </si>
-  <si>
-    <t>GetList()</t>
-  </si>
-  <si>
-    <t>GetSingleGroup()</t>
-  </si>
-  <si>
-    <t>Update()</t>
-  </si>
-  <si>
-    <t>Delete()</t>
-  </si>
-  <si>
-    <t>Pisteet: int</t>
-  </si>
-  <si>
     <t>int/10</t>
   </si>
   <si>
@@ -263,12 +221,6 @@
     <t>Tavoite suoritettu</t>
   </si>
   <si>
-    <t>Bool</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Tarkistaa onko tavoitteen pisteet saavutettu</t>
   </si>
   <si>
@@ -329,43 +281,157 @@
     <t>*tavoite_id</t>
   </si>
   <si>
-    <t>Hahmotunnus: str</t>
-  </si>
-  <si>
-    <t>Hahmonimi: str</t>
-  </si>
-  <si>
-    <t>Suoritetut tehtävät</t>
-  </si>
-  <si>
-    <t>Id: int</t>
-  </si>
-  <si>
-    <t>Tavoite: int</t>
-  </si>
-  <si>
-    <t>Suorituskerrat: int</t>
-  </si>
-  <si>
-    <t>Tavoite: str</t>
-  </si>
-  <si>
-    <t>Pvm: dt</t>
-  </si>
-  <si>
-    <t>1, *</t>
-  </si>
-  <si>
-    <t>1,*</t>
-  </si>
-  <si>
-    <t>TavoiteSuoritettu: bool</t>
-  </si>
-  <si>
-    <t>Animaatio: ?</t>
-  </si>
-  <si>
-    <t>YritysNimi: str</t>
+    <t>Linkki animaation sijaintiin</t>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t>www.linkki.fi/animaatiot/juoksu.aep</t>
+  </si>
+  <si>
+    <t>Uusi päivä</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Onko uusi päivä vai ei?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarkistaa, onko käyttäjä admin </t>
+  </si>
+  <si>
+    <t>Rekisteröintikoodi</t>
+  </si>
+  <si>
+    <t>Koodi, jolla pelaaja rekisteröityy yrityksensä pelialustalle</t>
+  </si>
+  <si>
+    <t>Pakollinen tehtävä</t>
+  </si>
+  <si>
+    <t>Tarkistaa, onko tehtävä pakollinen</t>
+  </si>
+  <si>
+    <t>Tavoitemäärä</t>
+  </si>
+  <si>
+    <t>Tehtävän tavoitemäärä</t>
+  </si>
+  <si>
+    <t>Viimeinen muokkaus</t>
+  </si>
+  <si>
+    <t>Tarkistaa, milloin pelaaja on viimeeksi suorittanut tehtävää</t>
+  </si>
+  <si>
+    <t>Hahmot</t>
+  </si>
+  <si>
+    <t>nimi: nvarchar</t>
+  </si>
+  <si>
+    <t>PK hahmo_id: int</t>
+  </si>
+  <si>
+    <t>animaatio1: nvarchar</t>
+  </si>
+  <si>
+    <t>animaatio2: nvarchar</t>
+  </si>
+  <si>
+    <t>animaatio3: nvarchar</t>
+  </si>
+  <si>
+    <t>Hae()</t>
+  </si>
+  <si>
+    <t>HaeKaikki()</t>
+  </si>
+  <si>
+    <t>Muokkaa()</t>
+  </si>
+  <si>
+    <t>Poista()</t>
+  </si>
+  <si>
+    <t>PK käyttäjä_id: int</t>
+  </si>
+  <si>
+    <t>FK hahmo_id: int</t>
+  </si>
+  <si>
+    <t>etunimi: nvarchar</t>
+  </si>
+  <si>
+    <t>sukunimi: nvarchar</t>
+  </si>
+  <si>
+    <t>salasana: nvarchar</t>
+  </si>
+  <si>
+    <t>sähköposti: nvarchar</t>
+  </si>
+  <si>
+    <t>rekisteröintikoodi: in</t>
+  </si>
+  <si>
+    <t>uusipäivä: bit</t>
+  </si>
+  <si>
+    <t>yritys: nvarchar</t>
+  </si>
+  <si>
+    <t>admin: bit</t>
+  </si>
+  <si>
+    <t>HaeRyhmä()</t>
+  </si>
+  <si>
+    <t>ValitutTehtävät</t>
+  </si>
+  <si>
+    <t>PK valitutteht_id: int</t>
+  </si>
+  <si>
+    <t>FK käyttäjä_id: int</t>
+  </si>
+  <si>
+    <t>FK tehtävä_id: int</t>
+  </si>
+  <si>
+    <t>pisteet: int</t>
+  </si>
+  <si>
+    <t>viimeinenmuokkaus: datetime</t>
+  </si>
+  <si>
+    <t>ei pidä paikkansa. Oikea er-malli suunnittelukuvastossa.</t>
+  </si>
+  <si>
+    <t>PK tehtävä_id: int</t>
+  </si>
+  <si>
+    <t>pistemäärä: int</t>
+  </si>
+  <si>
+    <t>tavoitemäärä: int</t>
+  </si>
+  <si>
+    <t>päivämäärä: datetime</t>
+  </si>
+  <si>
+    <t>pakollinen: bit</t>
+  </si>
+  <si>
+    <t>yrityskoodi: int</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -445,7 +511,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,8 +555,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -550,6 +634,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -561,7 +654,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,18 +670,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -602,9 +683,44 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1229,51 +1345,48 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604801</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Suora yhdysviiva 2">
+        <xdr:cNvPr id="17" name="Yhdistin: Kulma 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B54356-0BB7-4E2F-AE12-AFFB9466CF84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D06900B2-1947-4007-969C-57C6CCE86B0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1228725" y="962025"/>
-          <a:ext cx="1828800" cy="9525"/>
+        <a:xfrm rot="10800000">
+          <a:off x="3043201" y="296776"/>
+          <a:ext cx="1224000" cy="1332000"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1284,106 +1397,48 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>607201</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Suora yhdysviiva 6">
+        <xdr:cNvPr id="29" name="Yhdistin: Kulma 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C23F0CE-D645-4299-868A-F84C11FB3328}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1726CA-9CF4-4066-8346-6F4555BF192A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4257675" y="1152525"/>
-          <a:ext cx="1828800" cy="9525"/>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="6093601" y="502276"/>
+          <a:ext cx="612000" cy="936000"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Suora yhdysviiva 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B0316DD-4D2F-4165-8491-2882DFDDED78}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="1533525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1395,493 +1450,106 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Vinoneliö 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3615AA-0D14-4524-AA92-596282C40752}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="371475"/>
+          <a:ext cx="276225" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>607201</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Yhdistin: Kulma 9">
+        <xdr:cNvPr id="31" name="Yhdistin: Kulma 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9008C204-0973-4FF2-BD6F-AD49F8D43BDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4DA4F5-336A-4919-A968-44B7CDAAD30E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6105525" y="571500"/>
-          <a:ext cx="1219200" cy="571500"/>
+        <a:xfrm rot="10800000">
+          <a:off x="8532001" y="662251"/>
+          <a:ext cx="612000" cy="576000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Suora yhdysviiva 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7717D20-59E4-4E74-9BB9-49CDB3F37E27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4267200" y="3057525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Suora yhdysviiva 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E1CEC3-A659-408D-9F9C-70ED042D4045}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7305675" y="3438525"/>
-          <a:ext cx="1828800" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>487973</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Ryhmä 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F703A64B-380A-4F54-B31E-632D8969D62A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm rot="10800000">
-          <a:off x="9220200" y="942975"/>
-          <a:ext cx="411773" cy="2171700"/>
-          <a:chOff x="1312252" y="685800"/>
-          <a:chExt cx="411773" cy="2171700"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="16" name="Suora nuoliyhdysviiva 15">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A66396-EA1C-4393-A15B-4CD73BD3612C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1312252" y="2845777"/>
-            <a:ext cx="411773" cy="2199"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="18" name="Suora yhdysviiva 17">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC6A21D-F962-4570-AD3A-487F1C97FB4C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1319579" y="685800"/>
-            <a:ext cx="4396" cy="2171700"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>138479</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="22" name="Ryhmä 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83CC1DF2-2428-4AD5-A20B-212FA7573C5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3796079" y="771525"/>
-          <a:ext cx="433021" cy="2171700"/>
-          <a:chOff x="3796079" y="771525"/>
-          <a:chExt cx="433021" cy="2171700"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="9" name="Ryhmä 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A8993B-E1D4-428D-9082-1F977537141A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="3796079" y="771525"/>
-            <a:ext cx="411773" cy="2171700"/>
-            <a:chOff x="1312252" y="685800"/>
-            <a:chExt cx="411773" cy="2171700"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="11" name="Suora nuoliyhdysviiva 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16B39C1-E2A7-44A1-B3FC-DED636C7CF21}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1312252" y="2845777"/>
-              <a:ext cx="411773" cy="2199"/>
-            </a:xfrm>
-            <a:prstGeom prst="straightConnector1">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="13" name="Suora yhdysviiva 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA21815-F3CA-4F1C-A183-2C9C0C5FB0BE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1319579" y="685800"/>
-              <a:ext cx="4396" cy="2171700"/>
-            </a:xfrm>
-            <a:prstGeom prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-      </xdr:grpSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="4" name="Suora yhdysviiva 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A9A57D-9EA7-4D54-948E-2CC1C5E4AFAD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3800475" y="781050"/>
-            <a:ext cx="428625" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>43229</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>471854</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Suora yhdysviiva 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F887DB22-18CF-4A79-B6C3-B854C70BA33D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9187229" y="3105150"/>
-          <a:ext cx="428625" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
+        <a:lnRef idx="3">
           <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
           <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="2">
           <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -2193,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D048614-1B1B-4BED-86DE-CDA5E2BCD1F2}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +1872,7 @@
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="73.42578125" customWidth="1"/>
   </cols>
@@ -2240,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -2258,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2269,20 +1937,18 @@
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3">
         <v>30</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2290,22 +1956,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2313,21 +1976,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="3">
-        <v>6.5740740740740738E-2</v>
+      <c r="F5" s="16">
+        <v>43984</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2335,22 +1998,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2358,7 +2018,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -2376,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,7 +2044,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -2402,7 +2062,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,23 +2070,21 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3">
         <v>50</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2434,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2451,8 +2109,8 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>67</v>
+      <c r="H10" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2460,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -2471,14 +2129,14 @@
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>1234567890</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2486,7 +2144,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2497,14 +2155,14 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>987654321</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2512,23 +2170,23 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3">
         <v>150</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2536,16 +2194,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
+        <v>86</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2553,7 +2211,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -2571,7 +2229,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2579,98 +2237,178 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2">
         <v>30</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="2">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2">
+        <v>67890</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="A22" s="2">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="16">
+        <v>43992</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -2695,18 +2433,19 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" xr:uid="{480B066D-8DD9-4683-9ED8-6C2FC49271C4}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{0793E14C-77EC-4043-A5C9-ED6F6A97FA1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3ED8FE-25BB-46DF-9687-5EE052BFD54B}">
-  <dimension ref="D2:L18"/>
+  <dimension ref="D1:L18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,194 +2458,199 @@
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="2" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="22"/>
-      <c r="K2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" s="22"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="19"/>
-      <c r="E3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="21"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13"/>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>35</v>
+      <c r="E4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="15"/>
+        <v>71</v>
+      </c>
+      <c r="K9" s="7"/>
     </row>
     <row r="11" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="19"/>
-      <c r="E12" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="21"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="21"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="16" t="s">
+      <c r="E14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="16" t="s">
+      <c r="E15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="L15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2917,285 +2661,384 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B502A3A-5ACC-4FF4-88C3-BF4803BFC12F}">
-  <dimension ref="C1:P22"/>
+  <dimension ref="C1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H1" s="7"/>
-      <c r="I1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-      <c r="D3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="H3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="2">
+    <row r="1" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="24"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="21">
         <v>1</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="G4">
+      <c r="G3" s="20"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="32"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="21">
         <v>1</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="M4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="2" t="s">
+      <c r="L9" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="L5" s="26" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20">
+        <v>1</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H11" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="P11" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H12" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="P12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H13" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="P13" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H14" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="P14" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="P15" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H16" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="P16" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="H6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="M6" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="M7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="M8" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="M9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="M10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="M12" s="7"/>
-      <c r="N12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H13" s="7"/>
-      <c r="I13" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="M13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H14" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="M14" s="8" t="s">
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+    </row>
+    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H17" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="P17" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+    </row>
+    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H18" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="M15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="M16" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="M17" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="M18" s="8" t="s">
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H19" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" t="s">
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H22" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="M19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="M22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L2:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>